<commit_message>
Getting started with the basic
In this file you will find codes referring to: Identify operators;
Variable names;
Type of variables;
Code result;
Code analysis.
</commit_message>
<xml_diff>
--- a/Some Useful Codes/List of codes.xlsx
+++ b/Some Useful Codes/List of codes.xlsx
@@ -192,52 +192,52 @@
     <t>Code result</t>
   </si>
   <si>
-    <t xml:space="preserve">
+    <t>Code analysis</t>
+  </si>
+  <si>
+    <t>Is the number even or odd ?  &gt;  With this code the user can identify whether the number is even or odd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &gt;  This code can be used for validate whether the year is a leap year or not.</t>
+  </si>
+  <si>
+    <t>List_1_EX_6 - Sum operator   &gt; In this document, we have the code to make the sum of numbers.</t>
+  </si>
+  <si>
+    <t>List_1_EX_7 - Multiplication Operator  &gt; This document has the code to multiply numbers</t>
+  </si>
+  <si>
+    <t>Division operator    In this document you can find a code with division operation</t>
+  </si>
+  <si>
+    <t>Operador de divisão</t>
+  </si>
+  <si>
+    <t>Operador de multiplicação</t>
+  </si>
+  <si>
+    <t>Operador de subtração</t>
+  </si>
+  <si>
+    <t>Operator subtraction  This document has a code with subtraction operator.</t>
+  </si>
+  <si>
+    <t>Summing numbers reported by the user &gt; 
+In this code the user enters two numbers and the program sums the two.</t>
+  </si>
+  <si>
+    <t>Multiplying numbers reported by the user  &gt; In this document you find the code for muliplying numbers reported by the user.</t>
+  </si>
+  <si>
+    <t>With this list you can search for the code you need and identify quickly the name of the file you should download.</t>
+  </si>
+  <si>
+    <t>List of code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting started with the basics  &gt;
 In this file you will find codes referring to: Identify operators 
 </t>
-  </si>
-  <si>
-    <t>Code analysis</t>
-  </si>
-  <si>
-    <t>Is the number even or odd ?  &gt;  With this code the user can identify whether the number is even or odd.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  &gt;  This code can be used for validate whether the year is a leap year or not.</t>
-  </si>
-  <si>
-    <t>List_1_EX_6 - Sum operator   &gt; In this document, we have the code to make the sum of numbers.</t>
-  </si>
-  <si>
-    <t>List_1_EX_7 - Multiplication Operator  &gt; This document has the code to multiply numbers</t>
-  </si>
-  <si>
-    <t>Division operator    In this document you can find a code with division operation</t>
-  </si>
-  <si>
-    <t>Operador de divisão</t>
-  </si>
-  <si>
-    <t>Operador de multiplicação</t>
-  </si>
-  <si>
-    <t>Operador de subtração</t>
-  </si>
-  <si>
-    <t>Operator subtraction  This document has a code with subtraction operator.</t>
-  </si>
-  <si>
-    <t>Summing numbers reported by the user &gt; 
-In this code the user enters two numbers and the program sums the two.</t>
-  </si>
-  <si>
-    <t>Multiplying numbers reported by the user  &gt; In this document you find the code for muliplying numbers reported by the user.</t>
-  </si>
-  <si>
-    <t>With this list you can search for the code you need and identify quickly the name of the file you should download.</t>
-  </si>
-  <si>
-    <t>List of code</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,7 +633,7 @@
     <col min="3" max="3" width="56.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="110" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="128.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -670,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -693,7 +693,7 @@
         <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -744,7 +744,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -772,13 +772,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -789,13 +789,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -806,13 +806,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
@@ -829,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -846,7 +846,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -954,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1031,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6">

</xml_diff>